<commit_message>
built documentation for QA Scripts 5-10, added params_table function to index
</commit_message>
<xml_diff>
--- a/data/FMG_Tech_Tables.xlsx
+++ b/data/FMG_Tech_Tables.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FMG-Technical-Manual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{615B6C3E-2C1A-4332-B2AF-107534840708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{712FBC98-D58B-4887-8A24-9FE76A41AC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{0036D909-84D8-437D-AD81-9221A1AEED05}"/>
+    <workbookView xWindow="-15270" yWindow="7640" windowWidth="28800" windowHeight="15500" activeTab="7" xr2:uid="{0036D909-84D8-437D-AD81-9221A1AEED05}"/>
   </bookViews>
   <sheets>
     <sheet name="QA_Tool4" sheetId="1" r:id="rId1"/>
     <sheet name="QA_Tool3" sheetId="2" r:id="rId2"/>
     <sheet name="QA_Tool1" sheetId="12" r:id="rId3"/>
     <sheet name="QA_Tool2" sheetId="3" r:id="rId4"/>
-    <sheet name="ES_PrismPlot" sheetId="4" r:id="rId5"/>
-    <sheet name="ES_StandSpp" sheetId="5" r:id="rId6"/>
-    <sheet name="ES_StandNotes" sheetId="6" r:id="rId7"/>
-    <sheet name="FCOM_KEY" sheetId="7" r:id="rId8"/>
+    <sheet name="QA_Tool5" sheetId="4" r:id="rId5"/>
+    <sheet name="QA_Tool6" sheetId="5" r:id="rId6"/>
+    <sheet name="QA_Tool7" sheetId="6" r:id="rId7"/>
+    <sheet name="QA_Tool8" sheetId="7" r:id="rId8"/>
     <sheet name="QA_Scripts" sheetId="11" r:id="rId9"/>
     <sheet name="Py_Script_Tools" sheetId="8" r:id="rId10"/>
     <sheet name="USDA_Codes" sheetId="9" r:id="rId11"/>
@@ -47,173 +47,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="282">
-  <si>
-    <t>Field Name</t>
-  </si>
-  <si>
-    <t>Field Description</t>
-  </si>
-  <si>
-    <t>Field Type</t>
-  </si>
-  <si>
-    <t>OBJECTID</t>
-  </si>
-  <si>
-    <t>Object ID</t>
-  </si>
-  <si>
-    <t>SID</t>
-  </si>
-  <si>
-    <t>Unique stand identifier</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>AV_BA</t>
-  </si>
-  <si>
-    <t>Av. BA/Acre</t>
-  </si>
-  <si>
-    <t>AV_TPA</t>
-  </si>
-  <si>
-    <t>Av. TPA</t>
-  </si>
-  <si>
-    <t>NUM_TR</t>
-  </si>
-  <si>
-    <t># of count trees</t>
-  </si>
-  <si>
-    <t>Short integer</t>
-  </si>
-  <si>
-    <t>Community type code</t>
-  </si>
-  <si>
-    <t>POOL</t>
-  </si>
-  <si>
-    <t>Pool or river reach</t>
-  </si>
-  <si>
-    <t>COMP</t>
-  </si>
-  <si>
-    <t>Management compartment</t>
-  </si>
-  <si>
-    <t>UNIT</t>
-  </si>
-  <si>
-    <t>Management unit</t>
-  </si>
-  <si>
-    <t>SITE</t>
-  </si>
-  <si>
-    <t>Management site</t>
-  </si>
-  <si>
-    <t>PID</t>
-  </si>
-  <si>
-    <t>Unique plot identifier</t>
-  </si>
-  <si>
-    <t>Tree species</t>
-  </si>
-  <si>
-    <t>Tree DBH</t>
-  </si>
-  <si>
-    <t>MISC</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>COL_CREW</t>
-  </si>
-  <si>
-    <t>Collection crew</t>
-  </si>
-  <si>
-    <t>COL_DATE</t>
-  </si>
-  <si>
-    <t>Collection date</t>
-  </si>
-  <si>
-    <t>ArcGIS Database Key (auto-generated)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="252">
   <si>
     <t>TR_SP</t>
   </si>
   <si>
-    <t>TR_DIA</t>
-  </si>
-  <si>
-    <t>TR_CL</t>
-  </si>
-  <si>
-    <t>Tree canopy class</t>
-  </si>
-  <si>
-    <t>TR_HLTH</t>
-  </si>
-  <si>
-    <t>Tree health class</t>
-  </si>
-  <si>
     <t>MAST_TYPE</t>
   </si>
   <si>
-    <t>Tree mast type</t>
-  </si>
-  <si>
-    <t>IMP_VAL</t>
-  </si>
-  <si>
-    <t>Importance Value (300)</t>
-  </si>
-  <si>
-    <t>NOTE_BY</t>
-  </si>
-  <si>
-    <t>Note author</t>
-  </si>
-  <si>
-    <t>NOTE_DATE</t>
-  </si>
-  <si>
-    <t>Date of note</t>
-  </si>
-  <si>
-    <t>NOTE</t>
-  </si>
-  <si>
-    <t>Note field</t>
-  </si>
-  <si>
-    <t>COM_TYPE</t>
-  </si>
-  <si>
-    <t>Forest community type</t>
-  </si>
-  <si>
-    <t>CODE</t>
-  </si>
-  <si>
     <t>Tool Name</t>
   </si>
   <si>
@@ -838,9 +679,6 @@
     <t>Name of date field</t>
   </si>
   <si>
-    <t>Name of notes field</t>
-  </si>
-  <si>
     <t>Fixed plot feature class</t>
   </si>
   <si>
@@ -893,6 +731,78 @@
   </si>
   <si>
     <t>optional</t>
+  </si>
+  <si>
+    <t>fc_age</t>
+  </si>
+  <si>
+    <t>Age plot feature class</t>
+  </si>
+  <si>
+    <t>Name of tree diameter field</t>
+  </si>
+  <si>
+    <t>Name of tree height field</t>
+  </si>
+  <si>
+    <t>Name of tree year of origin field</t>
+  </si>
+  <si>
+    <t>Name of tree growth rate field</t>
+  </si>
+  <si>
+    <t>Species Field</t>
+  </si>
+  <si>
+    <t>DBH Field</t>
+  </si>
+  <si>
+    <t>Height Field</t>
+  </si>
+  <si>
+    <t>Year of Origin Field</t>
+  </si>
+  <si>
+    <t>Growth Rate Field</t>
+  </si>
+  <si>
+    <t>fc_center</t>
+  </si>
+  <si>
+    <t>Primary set of plot locations</t>
+  </si>
+  <si>
+    <t>center_plot_id_field</t>
+  </si>
+  <si>
+    <t>prism_plot_id_field</t>
+  </si>
+  <si>
+    <t>fc_fixed</t>
+  </si>
+  <si>
+    <t>fixed_plot_id_field</t>
+  </si>
+  <si>
+    <t>age_plot_id_field</t>
+  </si>
+  <si>
+    <t>Prism plot ID field</t>
+  </si>
+  <si>
+    <t>Plot Center ID Field</t>
+  </si>
+  <si>
+    <t>Fixed Plot ID Field</t>
+  </si>
+  <si>
+    <t>Name of field which flags plots for age tree collection</t>
+  </si>
+  <si>
+    <t>Flag Field</t>
+  </si>
+  <si>
+    <t>Age Plot ID Field</t>
   </si>
 </sst>
 </file>
@@ -1246,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60100A8C-9F9B-463C-BC65-4C6EEF006E71}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,170 +1167,170 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>211</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>214</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>215</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>281</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>225</v>
       </c>
       <c r="B12" t="s">
-        <v>262</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1445,82 +1355,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1540,640 +1450,640 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>186</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>138</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2193,10 +2103,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2204,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2212,7 +2122,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2220,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2228,7 +2138,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2236,7 +2146,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2244,7 +2154,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2252,7 +2162,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -2260,7 +2170,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -2268,7 +2178,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2276,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -2284,7 +2194,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -2292,7 +2202,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -2300,7 +2210,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -2308,7 +2218,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -2316,7 +2226,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -2324,7 +2234,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2247,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2348,142 +2258,142 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2508,86 +2418,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2613,58 +2523,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2675,383 +2585,408 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D1E1A2-D42B-4166-8BAF-05A5C779BCB3}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C16"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>238</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>224</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D14A75-6638-4ED2-B35C-62D406039211}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>239</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>229</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>189</v>
+      </c>
+      <c r="D8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB7BD7-190E-491A-B54C-E56BB01832A4}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>248</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3061,56 +2996,101 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C162C060-B266-4AD3-B727-63C97170D289}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>249</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3133,63 +3113,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>